<commit_message>
Added 3eme-1ere I classes
</commit_message>
<xml_diff>
--- a/Lesson_Names.xlsx
+++ b/Lesson_Names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\GitHub\Luxembourgish_Lycee_Classes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA9A064-0D94-4DE6-876C-E5E776C001B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83ED0FD4-82C8-4BA9-8509-DE25D52C0001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="2685" windowWidth="28800" windowHeight="15345" xr2:uid="{7A83D562-98D3-461B-AE3C-491BB9C6013F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="105">
   <si>
     <t>Original Name</t>
   </si>
@@ -315,6 +315,45 @@
   </si>
   <si>
     <t>Histo/Géo</t>
+  </si>
+  <si>
+    <t>Science de la programmation</t>
+  </si>
+  <si>
+    <t>Programmation</t>
+  </si>
+  <si>
+    <t>Communication média</t>
+  </si>
+  <si>
+    <t>ComMédia</t>
+  </si>
+  <si>
+    <t>Technologies appliquées et projets</t>
+  </si>
+  <si>
+    <t>TechApp</t>
+  </si>
+  <si>
+    <t>Maîtrise d'ouvrage</t>
+  </si>
+  <si>
+    <t>Ouvrage</t>
+  </si>
+  <si>
+    <t>Technologie</t>
+  </si>
+  <si>
+    <t>Technologie et innovations</t>
+  </si>
+  <si>
+    <t>Design graphique</t>
+  </si>
+  <si>
+    <t>Analyse et modélisation d'informations</t>
+  </si>
+  <si>
+    <t>Économie et finances</t>
   </si>
 </sst>
 </file>
@@ -687,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAFD0598-0CFE-4A19-87B1-A72EE293676A}">
-  <dimension ref="B3:C58"/>
+  <dimension ref="B3:C66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +757,7 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>83</v>
@@ -726,431 +765,495 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>60</v>
+        <v>104</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>24</v>
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>88</v>
+        <v>6</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>26</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>89</v>
+        <v>20</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>71</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>75</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>39</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>81</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>13</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C66" s="2" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B3:C5" xr:uid="{BAFD0598-0CFE-4A19-87B1-A72EE293676A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:C58">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:C66">
       <sortCondition ref="B3:B5"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Added multiple extra classique classes
</commit_message>
<xml_diff>
--- a/Lesson_Names.xlsx
+++ b/Lesson_Names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\GitHub\Luxembourgish_Lycee_Classes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7EA0F00-78DF-43D8-A746-9B0B10BDCAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB478B5-D926-40CE-8EBD-BA25B1E66761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="2685" windowWidth="28800" windowHeight="15345" xr2:uid="{7A83D562-98D3-461B-AE3C-491BB9C6013F}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15345" xr2:uid="{7A83D562-98D3-461B-AE3C-491BB9C6013F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="121">
   <si>
     <t>Original Name</t>
   </si>
@@ -381,6 +381,27 @@
   </si>
   <si>
     <t>Informatique/Projet</t>
+  </si>
+  <si>
+    <t>Arts</t>
+  </si>
+  <si>
+    <t>Technologie de l'information et de la communication</t>
+  </si>
+  <si>
+    <t>TechInfo/Com</t>
+  </si>
+  <si>
+    <t>Arts pluriels</t>
+  </si>
+  <si>
+    <t>Vie, société et religions</t>
+  </si>
+  <si>
+    <t>VieSoRel</t>
+  </si>
+  <si>
+    <t>Informatique appliquée</t>
   </si>
 </sst>
 </file>
@@ -753,16 +774,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAFD0598-0CFE-4A19-87B1-A72EE293676A}">
-  <dimension ref="B3:C71"/>
+  <dimension ref="B3:C76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -816,511 +837,551 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>41</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>25</v>
+        <v>108</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>94</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>102</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>58</v>
+        <v>104</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>62</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>15</v>
+        <v>68</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" t="s">
-        <v>2</v>
+        <v>79</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>65</v>
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>112</v>
+        <v>46</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>113</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>17</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>93</v>
+        <v>21</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>107</v>
-      </c>
-      <c r="C61" t="s">
-        <v>107</v>
+        <v>87</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>5</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>89</v>
+        <v>29</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>75</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>76</v>
+        <v>107</v>
+      </c>
+      <c r="C64" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>39</v>
+        <v>78</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
+        <v>96</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>39</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>81</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>70</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
         <v>13</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C75" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>118</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B3:C5" xr:uid="{BAFD0598-0CFE-4A19-87B1-A72EE293676A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:C71">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:C76">
       <sortCondition ref="B3:B5"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Finished adding all classique classes
</commit_message>
<xml_diff>
--- a/Lesson_Names.xlsx
+++ b/Lesson_Names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micfe484\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\GitHub\Luxembourgish_Lycee_Classes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3737BE2-838D-40FB-B211-5814834CF894}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEA17FC-2D6D-4635-8013-4C2368730827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7890" xr2:uid="{7A83D562-98D3-461B-AE3C-491BB9C6013F}"/>
+    <workbookView xWindow="14460" yWindow="3840" windowWidth="21420" windowHeight="15345" xr2:uid="{7A83D562-98D3-461B-AE3C-491BB9C6013F}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="140">
   <si>
     <t>Original Name</t>
   </si>
@@ -433,6 +444,21 @@
   </si>
   <si>
     <t>Géographie territoriale</t>
+  </si>
+  <si>
+    <t>Communication média / pratique des médias</t>
+  </si>
+  <si>
+    <t>Pratique des médias</t>
+  </si>
+  <si>
+    <t>Pratique</t>
+  </si>
+  <si>
+    <t>Littérature</t>
+  </si>
+  <si>
+    <t>Littérature comparée</t>
   </si>
 </sst>
 </file>
@@ -493,7 +519,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -509,7 +535,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -805,13 +831,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAFD0598-0CFE-4A19-87B1-A72EE293676A}">
-  <dimension ref="B3:C84"/>
+  <dimension ref="B3:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.7109375" bestFit="1" customWidth="1"/>
@@ -940,39 +966,39 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>32</v>
+        <v>135</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>120</v>
-      </c>
-      <c r="C20" t="s">
-        <v>120</v>
+        <v>26</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>63</v>
+        <v>120</v>
+      </c>
+      <c r="C21" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>63</v>
@@ -980,71 +1006,71 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>126</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>72</v>
+        <v>119</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>29</v>
@@ -1052,127 +1078,127 @@
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>123</v>
+        <v>57</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>124</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>15</v>
+        <v>123</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>8</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>127</v>
+        <v>62</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>68</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>2</v>
-      </c>
-      <c r="C42" t="s">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>133</v>
+        <v>7</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>134</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>65</v>
+        <v>133</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>23</v>
@@ -1180,39 +1206,39 @@
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>35</v>
+        <v>89</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>87</v>
+        <v>33</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>34</v>
@@ -1220,263 +1246,287 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>111</v>
+        <v>54</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>112</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>97</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>98</v>
+        <v>139</v>
+      </c>
+      <c r="C60" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>92</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>106</v>
-      </c>
-      <c r="C71" t="s">
-        <v>106</v>
+        <v>86</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>11</v>
+        <v>91</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>5</v>
+        <v>92</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>74</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>75</v>
+        <v>106</v>
+      </c>
+      <c r="C74" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>129</v>
+        <v>11</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>130</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>114</v>
+        <v>74</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>37</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
+        <v>80</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>69</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
         <v>117</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C87" s="2" t="s">
         <v>122</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B3:C5" xr:uid="{BAFD0598-0CFE-4A19-87B1-A72EE293676A}">
-    <sortState ref="B4:C84">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:C87">
       <sortCondition ref="B3:B5"/>
     </sortState>
   </autoFilter>

</xml_diff>